<commit_message>
added cards to members app
</commit_message>
<xml_diff>
--- a/kbfc/members/members.xlsx
+++ b/kbfc/members/members.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shodeshp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shodeshp\Documents\Learning\kbfc\kbfc\members\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55FAAF1-E038-4E7E-BA98-B1EFCB49C3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828D2718-AA6E-499F-A80C-0F9D0701724C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{8D629BC8-D947-4AC1-8960-499C478CAA2A}"/>
   </bookViews>
@@ -22,6 +22,9 @@
     <sheet name="ProfessionalPlayerNames" sheetId="6" r:id="rId7"/>
     <sheet name="Foot" sheetId="8" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Memberlist!$A$1:$N$21</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="207">
   <si>
     <t>Company</t>
   </si>
@@ -279,39 +282,6 @@
     <t>upload/009.JPG</t>
   </si>
   <si>
-    <t>upload/0010.JPG</t>
-  </si>
-  <si>
-    <t>upload/0011.JPG</t>
-  </si>
-  <si>
-    <t>upload/0012.JPG</t>
-  </si>
-  <si>
-    <t>upload/0013.JPG</t>
-  </si>
-  <si>
-    <t>upload/0014.JPG</t>
-  </si>
-  <si>
-    <t>upload/0015.JPG</t>
-  </si>
-  <si>
-    <t>upload/0016.JPG</t>
-  </si>
-  <si>
-    <t>upload/0017.JPG</t>
-  </si>
-  <si>
-    <t>upload/0018.JPG</t>
-  </si>
-  <si>
-    <t>upload/0019.JPG</t>
-  </si>
-  <si>
-    <t>upload/0020.JPG</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
@@ -498,9 +468,6 @@
     <t>46/167, Zeus Lane, 6th Lane, Devil May Cry Nagar, Kolhapur - 400074.</t>
   </si>
   <si>
-    <t>Midfielder</t>
-  </si>
-  <si>
     <t>Profession</t>
   </si>
   <si>
@@ -667,6 +634,39 @@
   </si>
   <si>
     <t>Foot</t>
+  </si>
+  <si>
+    <t>upload/010.JPG</t>
+  </si>
+  <si>
+    <t>upload/011.JPG</t>
+  </si>
+  <si>
+    <t>upload/012.JPG</t>
+  </si>
+  <si>
+    <t>upload/013.JPG</t>
+  </si>
+  <si>
+    <t>upload/014.JPG</t>
+  </si>
+  <si>
+    <t>upload/015.JPG</t>
+  </si>
+  <si>
+    <t>upload/016.JPG</t>
+  </si>
+  <si>
+    <t>upload/017.JPG</t>
+  </si>
+  <si>
+    <t>upload/018.JPG</t>
+  </si>
+  <si>
+    <t>upload/019.JPG</t>
+  </si>
+  <si>
+    <t>upload/020.JPG</t>
   </si>
 </sst>
 </file>
@@ -1278,7 +1278,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1350,22 +1350,22 @@
         <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="G2" s="2">
         <v>31060.3125</v>
       </c>
       <c r="H2" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -1374,16 +1374,16 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="N2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1394,16 +1394,16 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G3" s="2">
         <v>34731.681944444441</v>
@@ -1418,16 +1418,16 @@
         <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="N3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1438,16 +1438,16 @@
         <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="G4" s="2">
         <v>31099.839583333334</v>
@@ -1462,16 +1462,16 @@
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1482,16 +1482,16 @@
         <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="G5" s="2">
         <v>34488.88958333333</v>
@@ -1506,16 +1506,16 @@
         <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="N5" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1526,16 +1526,16 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E6" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G6" s="2">
         <v>33966.693749999999</v>
@@ -1550,16 +1550,16 @@
         <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="L6" t="s">
         <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="N6" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1570,22 +1570,22 @@
         <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G7" s="2">
         <v>33619.384027777778</v>
       </c>
       <c r="H7" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="I7" t="s">
         <v>29</v>
@@ -1594,16 +1594,16 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="N7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1614,16 +1614,16 @@
         <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G8" s="2">
         <v>34061.568749999999</v>
@@ -1638,16 +1638,16 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="L8" t="s">
         <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="N8" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1658,16 +1658,16 @@
         <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="G9" s="2">
         <v>33204.515972222223</v>
@@ -1682,16 +1682,16 @@
         <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="L9" t="s">
         <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="N9" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1702,16 +1702,16 @@
         <v>77</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F10" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G10" s="2">
         <v>34647.415277777778</v>
@@ -1726,16 +1726,16 @@
         <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="L10" t="s">
         <v>9</v>
       </c>
       <c r="M10" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="N10" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1743,19 +1743,19 @@
         <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F11" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="G11" s="2">
         <v>32238.613888888889</v>
@@ -1770,16 +1770,16 @@
         <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="N11" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1787,25 +1787,25 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E12" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="G12" s="2">
         <v>33003.909722222219</v>
       </c>
       <c r="H12" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="I12" t="s">
         <v>33</v>
@@ -1814,16 +1814,16 @@
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="N12" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1831,19 +1831,19 @@
         <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="G13" s="2">
         <v>32838.240277777775</v>
@@ -1858,16 +1858,16 @@
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="L13" t="s">
         <v>12</v>
       </c>
       <c r="M13" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="N13" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1875,19 +1875,19 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="G14" s="2">
         <v>33574.056944444441</v>
@@ -1902,16 +1902,16 @@
         <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="L14" t="s">
         <v>13</v>
       </c>
       <c r="M14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="N14" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1919,19 +1919,19 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="F15" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G15" s="2">
         <v>34566.943055555559</v>
@@ -1946,16 +1946,16 @@
         <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="L15" t="s">
         <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="N15" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -1963,19 +1963,19 @@
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2">
         <v>33396.081944444442</v>
@@ -1990,16 +1990,16 @@
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="L16" t="s">
         <v>15</v>
       </c>
       <c r="M16" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="N16" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -2007,25 +2007,25 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G17" s="2">
         <v>32508.545833333334</v>
       </c>
       <c r="H17" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="I17" t="s">
         <v>26</v>
@@ -2034,16 +2034,16 @@
         <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="L17" t="s">
         <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="N17" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -2051,19 +2051,19 @@
         <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="G18" s="2">
         <v>32985.886111111111</v>
@@ -2078,16 +2078,16 @@
         <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="L18" t="s">
         <v>6</v>
       </c>
       <c r="M18" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="N18" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2095,19 +2095,19 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G19" s="2">
         <v>32103.816666666666</v>
@@ -2122,16 +2122,16 @@
         <v>25</v>
       </c>
       <c r="K19" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="L19" t="s">
         <v>7</v>
       </c>
       <c r="M19" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="N19" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2139,19 +2139,19 @@
         <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="G20" s="2">
         <v>32148.513888888891</v>
@@ -2166,16 +2166,16 @@
         <v>26</v>
       </c>
       <c r="K20" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="L20" t="s">
         <v>8</v>
       </c>
       <c r="M20" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="N20" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2183,19 +2183,19 @@
         <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="G21" s="2">
         <v>33565.951388888891</v>
@@ -2210,16 +2210,16 @@
         <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="L21" t="s">
         <v>9</v>
       </c>
       <c r="M21" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="N21" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2245,67 +2245,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2325,107 +2325,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2445,107 +2445,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2565,17 +2565,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed static file path
</commit_message>
<xml_diff>
--- a/kbfc/members/members.xlsx
+++ b/kbfc/members/members.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shodeshp\Documents\Learning\kbfc\kbfc\members\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828D2718-AA6E-499F-A80C-0F9D0701724C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F8E60-061B-4C73-872A-9783008DBBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{8D629BC8-D947-4AC1-8960-499C478CAA2A}"/>
   </bookViews>
@@ -255,33 +255,6 @@
     <t>Lucia Hancock</t>
   </si>
   <si>
-    <t>upload/001.JPG</t>
-  </si>
-  <si>
-    <t>upload/002.JPG</t>
-  </si>
-  <si>
-    <t>upload/003.JPG</t>
-  </si>
-  <si>
-    <t>upload/004.JPG</t>
-  </si>
-  <si>
-    <t>upload/005.JPG</t>
-  </si>
-  <si>
-    <t>upload/006.JPG</t>
-  </si>
-  <si>
-    <t>upload/007.JPG</t>
-  </si>
-  <si>
-    <t>upload/008.JPG</t>
-  </si>
-  <si>
-    <t>upload/009.JPG</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
@@ -636,37 +609,64 @@
     <t>Foot</t>
   </si>
   <si>
-    <t>upload/010.JPG</t>
-  </si>
-  <si>
-    <t>upload/011.JPG</t>
-  </si>
-  <si>
-    <t>upload/012.JPG</t>
-  </si>
-  <si>
-    <t>upload/013.JPG</t>
-  </si>
-  <si>
-    <t>upload/014.JPG</t>
-  </si>
-  <si>
-    <t>upload/015.JPG</t>
-  </si>
-  <si>
-    <t>upload/016.JPG</t>
-  </si>
-  <si>
-    <t>upload/017.JPG</t>
-  </si>
-  <si>
-    <t>upload/018.JPG</t>
-  </si>
-  <si>
-    <t>upload/019.JPG</t>
-  </si>
-  <si>
-    <t>upload/020.JPG</t>
+    <t>static/upload/001.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/002.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/003.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/004.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/005.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/006.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/007.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/008.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/009.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/010.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/011.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/012.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/013.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/014.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/015.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/016.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/017.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/018.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/019.JPG</t>
+  </si>
+  <si>
+    <t>static/upload/020.JPG</t>
   </si>
 </sst>
 </file>
@@ -1278,13 +1278,13 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="7" customWidth="1"/>
@@ -1347,19 +1347,19 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G2" s="2">
         <v>31060.3125</v>
@@ -1374,16 +1374,16 @@
         <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L2" t="s">
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="N2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -1391,19 +1391,19 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" t="s">
-        <v>79</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G3" s="2">
         <v>34731.681944444441</v>
@@ -1418,16 +1418,16 @@
         <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="L3" t="s">
         <v>2</v>
       </c>
       <c r="M3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="N3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1435,19 +1435,19 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G4" s="2">
         <v>31099.839583333334</v>
@@ -1462,16 +1462,16 @@
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="N4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1479,19 +1479,19 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="G5" s="2">
         <v>34488.88958333333</v>
@@ -1506,16 +1506,16 @@
         <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="L5" t="s">
         <v>4</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="N5" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1523,19 +1523,19 @@
         <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>191</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G6" s="2">
         <v>33966.693749999999</v>
@@ -1550,16 +1550,16 @@
         <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="L6" t="s">
         <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="N6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1567,19 +1567,19 @@
         <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2">
         <v>33619.384027777778</v>
@@ -1594,16 +1594,16 @@
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="L7" t="s">
         <v>6</v>
       </c>
       <c r="M7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="N7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1611,19 +1611,19 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="G8" s="2">
         <v>34061.568749999999</v>
@@ -1638,16 +1638,16 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="L8" t="s">
         <v>7</v>
       </c>
       <c r="M8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="N8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1655,19 +1655,19 @@
         <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="G9" s="2">
         <v>33204.515972222223</v>
@@ -1682,16 +1682,16 @@
         <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="L9" t="s">
         <v>8</v>
       </c>
       <c r="M9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="N9" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1699,19 +1699,19 @@
         <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G10" s="2">
         <v>34647.415277777778</v>
@@ -1726,16 +1726,16 @@
         <v>29</v>
       </c>
       <c r="K10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="L10" t="s">
         <v>9</v>
       </c>
       <c r="M10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="N10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -1746,16 +1746,16 @@
         <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G11" s="2">
         <v>32238.613888888889</v>
@@ -1770,16 +1770,16 @@
         <v>28</v>
       </c>
       <c r="K11" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="L11" t="s">
         <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="N11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -1790,16 +1790,16 @@
         <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G12" s="2">
         <v>33003.909722222219</v>
@@ -1814,16 +1814,16 @@
         <v>30</v>
       </c>
       <c r="K12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="L12" t="s">
         <v>11</v>
       </c>
       <c r="M12" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="N12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -1834,16 +1834,16 @@
         <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="G13" s="2">
         <v>32838.240277777775</v>
@@ -1858,16 +1858,16 @@
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="L13" t="s">
         <v>12</v>
       </c>
       <c r="M13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="N13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -1878,16 +1878,16 @@
         <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G14" s="2">
         <v>33574.056944444441</v>
@@ -1902,16 +1902,16 @@
         <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="L14" t="s">
         <v>13</v>
       </c>
       <c r="M14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="N14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -1922,16 +1922,16 @@
         <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G15" s="2">
         <v>34566.943055555559</v>
@@ -1946,16 +1946,16 @@
         <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="L15" t="s">
         <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="N15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -1966,16 +1966,16 @@
         <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="G16" s="2">
         <v>33396.081944444442</v>
@@ -1990,16 +1990,16 @@
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="L16" t="s">
         <v>15</v>
       </c>
       <c r="M16" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="N16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -2010,16 +2010,16 @@
         <v>202</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G17" s="2">
         <v>32508.545833333334</v>
@@ -2034,16 +2034,16 @@
         <v>18</v>
       </c>
       <c r="K17" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="L17" t="s">
         <v>16</v>
       </c>
       <c r="M17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="N17" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -2054,16 +2054,16 @@
         <v>203</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E18" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="F18" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="G18" s="2">
         <v>32985.886111111111</v>
@@ -2078,16 +2078,16 @@
         <v>19</v>
       </c>
       <c r="K18" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="L18" t="s">
         <v>6</v>
       </c>
       <c r="M18" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="N18" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2098,16 +2098,16 @@
         <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="G19" s="2">
         <v>32103.816666666666</v>
@@ -2122,16 +2122,16 @@
         <v>25</v>
       </c>
       <c r="K19" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L19" t="s">
         <v>7</v>
       </c>
       <c r="M19" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="N19" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2142,16 +2142,16 @@
         <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="G20" s="2">
         <v>32148.513888888891</v>
@@ -2166,16 +2166,16 @@
         <v>26</v>
       </c>
       <c r="K20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="L20" t="s">
         <v>8</v>
       </c>
       <c r="M20" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="N20" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2186,16 +2186,16 @@
         <v>206</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E21" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F21" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G21" s="2">
         <v>33565.951388888891</v>
@@ -2210,16 +2210,16 @@
         <v>27</v>
       </c>
       <c r="K21" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="L21" t="s">
         <v>9</v>
       </c>
       <c r="M21" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="N21" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2230,6 +2230,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2245,67 +2246,67 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2325,107 +2326,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2445,107 +2446,107 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2565,17 +2566,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>